<commit_message>
Corrijo puerto dinámico y agrego logs de depuración
</commit_message>
<xml_diff>
--- a/static/exportados/empleados_exportados.xlsx
+++ b/static/exportados/empleados_exportados.xlsx
@@ -5763,7 +5763,11 @@
           <t>2317577632</t>
         </is>
       </c>
-      <c r="N74" t="inlineStr"/>
+      <c r="N74" t="inlineStr">
+        <is>
+          <t>empleado</t>
+        </is>
+      </c>
       <c r="O74" t="inlineStr"/>
       <c r="P74" t="inlineStr"/>
       <c r="Q74" t="inlineStr"/>

</xml_diff>

<commit_message>
Actualización automática - 2025-07-30 13:03
</commit_message>
<xml_diff>
--- a/static/exportados/empleados_exportados.xlsx
+++ b/static/exportados/empleados_exportados.xlsx
@@ -984,7 +984,7 @@
       </c>
       <c r="O7" t="inlineStr"/>
       <c r="P7" t="n">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="Q7" t="inlineStr"/>
       <c r="R7" t="inlineStr"/>
@@ -1760,7 +1760,7 @@
       </c>
       <c r="O17" t="inlineStr"/>
       <c r="P17" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="Q17" t="inlineStr"/>
       <c r="R17" t="inlineStr"/>
@@ -2276,7 +2276,7 @@
       </c>
       <c r="O24" t="inlineStr"/>
       <c r="P24" t="n">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="Q24" t="inlineStr"/>
       <c r="R24" t="inlineStr"/>
@@ -2350,7 +2350,7 @@
       </c>
       <c r="O25" t="inlineStr"/>
       <c r="P25" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="Q25" t="inlineStr"/>
       <c r="R25" t="inlineStr"/>
@@ -2804,7 +2804,7 @@
       </c>
       <c r="O31" t="inlineStr"/>
       <c r="P31" t="n">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="Q31" t="inlineStr"/>
       <c r="R31" t="inlineStr"/>
@@ -2952,7 +2952,7 @@
       </c>
       <c r="O33" t="inlineStr"/>
       <c r="P33" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="Q33" t="inlineStr"/>
       <c r="R33" t="inlineStr"/>
@@ -3408,7 +3408,7 @@
       </c>
       <c r="O39" t="inlineStr"/>
       <c r="P39" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="Q39" t="inlineStr"/>
       <c r="R39" t="inlineStr"/>
@@ -3482,7 +3482,7 @@
       </c>
       <c r="O40" t="inlineStr"/>
       <c r="P40" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="Q40" t="inlineStr"/>
       <c r="R40" t="inlineStr"/>
@@ -3802,7 +3802,7 @@
       </c>
       <c r="O44" t="inlineStr"/>
       <c r="P44" t="n">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="Q44" t="inlineStr"/>
       <c r="R44" t="inlineStr"/>
@@ -6358,7 +6358,7 @@
       </c>
       <c r="O77" t="inlineStr"/>
       <c r="P77" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="Q77" t="inlineStr"/>
       <c r="R77" t="inlineStr"/>

</xml_diff>